<commit_message>
Weitere Vorbereitungen für den 2015er launch
</commit_message>
<xml_diff>
--- a/src/main/resources/kegelmeisterschaft/service/importer/2015/clubs.xlsx
+++ b/src/main/resources/kegelmeisterschaft/service/importer/2015/clubs.xlsx
@@ -789,7 +789,7 @@
         <v>32</v>
       </c>
       <c s="1" r="G10">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="11">
@@ -829,7 +829,7 @@
         <v>38</v>
       </c>
       <c s="1" r="G12">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="13">
@@ -849,7 +849,7 @@
         <v>41</v>
       </c>
       <c s="1" r="G13">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="14">
@@ -929,7 +929,7 @@
         <v>53</v>
       </c>
       <c s="1" r="G17">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="18">
@@ -1029,7 +1029,7 @@
         <v>68</v>
       </c>
       <c s="1" r="G22">
-        <v>4.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="23">

</xml_diff>